<commit_message>
Add models Item, RedressKit and RedressKitConsist
</commit_message>
<xml_diff>
--- a/bd_welltec.xlsx
+++ b/bd_welltec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t xml:space="preserve">Справочники</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t xml:space="preserve">Service Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -207,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,6 +237,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,7 +374,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -433,7 +453,6 @@
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
@@ -556,44 +575,62 @@
       <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="0"/>
+      <c r="D28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="0"/>
+      <c r="D29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="0"/>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="0"/>
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3" t="s">
@@ -602,7 +639,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +649,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>